<commit_message>
Added @property decorator to fullstring, identifier and keynotes methods.
</commit_message>
<xml_diff>
--- a/Test/testfile2.xlsx
+++ b/Test/testfile2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="81">
   <si>
     <t>General</t>
   </si>
@@ -68,12 +68,21 @@
     <t>Existing 2</t>
   </si>
   <si>
+    <t>E0003</t>
+  </si>
+  <si>
+    <t>&lt;Empty&gt;</t>
+  </si>
+  <si>
     <t>N0001</t>
   </si>
   <si>
     <t>New 1</t>
   </si>
   <si>
+    <t>N0002</t>
+  </si>
+  <si>
     <t>SITE</t>
   </si>
   <si>
@@ -158,13 +167,13 @@
     <t>D0201</t>
   </si>
   <si>
-    <t>Demo Floor 1</t>
+    <t>DEMO FLOOR 1</t>
   </si>
   <si>
     <t>D0202</t>
   </si>
   <si>
-    <t>&lt;Empty&gt;</t>
+    <t>&lt;EMPTY&gt;</t>
   </si>
   <si>
     <t>E0201</t>
@@ -182,6 +191,12 @@
     <t>E0203</t>
   </si>
   <si>
+    <t>E0204</t>
+  </si>
+  <si>
+    <t>EXISTING FLOOR AND FINISH TO REMAIN U.O.N.</t>
+  </si>
+  <si>
     <t>N0201</t>
   </si>
   <si>
@@ -227,10 +242,10 @@
     <t>D0401</t>
   </si>
   <si>
-    <t>Demo 1</t>
-  </si>
-  <si>
     <t>D0402</t>
+  </si>
+  <si>
+    <t>D0403</t>
   </si>
   <si>
     <t>E0401</t>
@@ -606,7 +621,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -716,71 +731,71 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="5" t="s">
-        <v>12</v>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="2" t="s">
-        <v>19</v>
+      <c r="C19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" t="n">
-        <v>1</v>
+      <c r="A21" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" t="s">
-        <v>9</v>
+      <c r="C23" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="C24" t="n">
         <v>1</v>
@@ -788,13 +803,13 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" t="n">
-        <v>1</v>
+      <c r="C25" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -802,18 +817,18 @@
         <v>29</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" t="s">
-        <v>9</v>
+        <v>30</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" t="n">
         <v>1</v>
@@ -821,51 +836,51 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" t="n">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="C28" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" t="n">
-        <v>1</v>
-      </c>
-    </row>
     <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" t="n">
-        <v>1</v>
+      <c r="A33" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -873,45 +888,45 @@
         <v>36</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C34" t="n">
         <v>1</v>
       </c>
     </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1</v>
+      </c>
+    </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="6" t="s">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" t="n">
+      <c r="C36" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" t="n">
-        <v>1</v>
+      <c r="A38" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="C39" t="n">
         <v>1</v>
@@ -922,7 +937,7 @@
         <v>42</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C40" t="n">
         <v>1</v>
@@ -930,10 +945,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C41" t="n">
         <v>1</v>
@@ -941,274 +956,291 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C42" t="n">
         <v>1</v>
       </c>
     </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1</v>
+      </c>
+    </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="2" t="s">
-        <v>45</v>
+      <c r="A44" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C46" t="n">
+      <c r="A46" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C47" t="n">
+    <row r="49" spans="1:3">
+      <c r="A49" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C50" t="n">
-        <v>2</v>
-      </c>
-    </row>
     <row r="51" spans="1:3">
-      <c r="A51" t="s">
-        <v>52</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C51" t="n">
-        <v>2</v>
+      <c r="A51" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="C52" t="n">
         <v>2</v>
       </c>
     </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" t="n">
+        <v>2</v>
+      </c>
+    </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="5" t="s">
-        <v>12</v>
+      <c r="A54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="6" t="s">
-        <v>55</v>
+      <c r="A55" t="s">
+        <v>58</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C55" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C56" t="s">
+    <row r="57" spans="1:3">
+      <c r="A57" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C59" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C57" t="n">
+    <row r="60" spans="1:3">
+      <c r="A60" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B61" s="4" t="s">
+    <row r="62" spans="1:3">
+      <c r="A62" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C61" t="n">
+      <c r="C64" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B62" s="4" t="s">
+    <row r="65" spans="1:3">
+      <c r="A65" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C62" t="n">
+      <c r="C65" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C63" t="n">
+    <row r="66" spans="1:3">
+      <c r="A66" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" t="s">
-        <v>63</v>
-      </c>
-      <c r="B66" s="4" t="s">
+    <row r="68" spans="1:3">
+      <c r="A68" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C69" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
-      <c r="A67" t="s">
-        <v>64</v>
-      </c>
-      <c r="B67" s="4" t="s">
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="C67" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="C70" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C71" t="n">
+    <row r="72" spans="1:3">
+      <c r="A72" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C73" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C75" t="n">
+      <c r="A74" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C74" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B76" s="4" t="s">
+    <row r="79" spans="1:3">
+      <c r="A79" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B79" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C79" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
-        <v>72</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C79" t="n">
-        <v>4</v>
-      </c>
-    </row>
     <row r="80" spans="1:3">
-      <c r="A80" t="s">
-        <v>73</v>
+      <c r="A80" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C80" t="n">
         <v>4</v>
@@ -1220,22 +1252,22 @@
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="6" t="s">
-        <v>74</v>
+      <c r="A83" t="s">
+        <v>77</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C83" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="6" t="s">
-        <v>75</v>
+      <c r="A84" t="s">
+        <v>78</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C84" t="n">
         <v>4</v>
@@ -1243,6 +1275,33 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C87" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C88" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1250,20 +1309,20 @@
   <mergeCells count="16">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A76:C76"/>
     <mergeCell ref="A82:C82"/>
     <mergeCell ref="A86:C86"/>
+    <mergeCell ref="A90:C90"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>